<commit_message>
Fix pricing api issue for china reigons, #1
</commit_message>
<xml_diff>
--- a/source/soca/cluster_analytics/price.xlsx
+++ b/source/soca/cluster_analytics/price.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jieding/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jieding/Documents/python-code/scale-out-computing-on-aws-china2.5/source/soca/cluster_analytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B7BE8A-BBA5-0C4B-A391-2DAD95E3AE6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D874A6A6-10E5-5042-A978-5AB6F5348A2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15880" activeTab="1" xr2:uid="{D1077547-9E19-0D4F-820F-DECDD58800E0}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15880" xr2:uid="{D1077547-9E19-0D4F-820F-DECDD58800E0}"/>
   </bookViews>
   <sheets>
     <sheet name="price" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -788,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7EDB6A-27A1-BC47-9A40-B9D9669940B0}">
   <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -2410,16 +2409,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3B97D9-FC35-E84E-A6CC-E3622E0DF8BD}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>